<commit_message>
c-model: add NVDLA power/area numbers
</commit_message>
<xml_diff>
--- a/c-model/area_power.xlsx
+++ b/c-model/area_power.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{F8DFADE6-D759-488F-8BD9-B433D2CD2F70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1B5F33-CA35-4344-BBB3-A88556229201}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1335" windowWidth="20730" windowHeight="11160" xr2:uid="{B4A96ED6-F37D-4104-88B0-F12BE89ED4ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{B4A96ED6-F37D-4104-88B0-F12BE89ED4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>accelerator</t>
   </si>
@@ -49,6 +54,12 @@
   </si>
   <si>
     <t>DECADES accelerators: area and power estimates</t>
+  </si>
+  <si>
+    <t>nvdla</t>
+  </si>
+  <si>
+    <t>sdp</t>
   </si>
 </sst>
 </file>
@@ -172,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -192,43 +203,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -551,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523FD97C-F56A-4138-AC1D-4D3D8891FEA4}">
-  <dimension ref="B1:I7"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,168 +571,196 @@
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="18">
+      <c r="C3" s="19"/>
+      <c r="D3" s="12">
         <v>32</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="13">
+        <v>16</v>
+      </c>
+      <c r="F3" s="13">
         <v>14</v>
       </c>
-      <c r="F3" s="19">
+      <c r="G3" s="13">
         <v>5</v>
       </c>
-      <c r="G3" s="19">
+      <c r="H3" s="13">
         <v>32</v>
       </c>
-      <c r="H3" s="19">
+      <c r="I3" s="13">
+        <v>16</v>
+      </c>
+      <c r="J3" s="13">
         <v>14</v>
       </c>
-      <c r="I3" s="15">
+      <c r="K3" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>54288</v>
       </c>
-      <c r="E4" s="2">
-        <f>D4*(E$3/$D$3)^2</f>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <f>D4*(F$3/$D$3)^2</f>
         <v>10391.0625</v>
       </c>
-      <c r="F4" s="2">
-        <f>$D4*(F$3/$D$3)^2</f>
+      <c r="G4" s="2">
+        <f>$D4*(G$3/$D$3)^2</f>
         <v>1325.390625</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>34</v>
       </c>
-      <c r="H4" s="2">
-        <f>G4*(H$3/$G$3)^2</f>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <f>H4*(J$3/$H$3)^2</f>
         <v>6.5078125</v>
       </c>
-      <c r="I4" s="3">
-        <f>G4*(I$3/$G$3)^2</f>
+      <c r="K4" s="3">
+        <f>H4*(K$3/$H$3)^2</f>
         <v>0.830078125</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="4">
         <v>200000</v>
       </c>
-      <c r="E5" s="5">
-        <f>D5*(E$3/$D$3)^2</f>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <f>D5*(F$3/$D$3)^2</f>
         <v>38281.25</v>
       </c>
-      <c r="F5" s="5">
-        <f>$D5*(F$3/$D$3)^2</f>
+      <c r="G5" s="5">
+        <f>$D5*(G$3/$D$3)^2</f>
         <v>4882.8125</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <v>400</v>
       </c>
-      <c r="H5" s="5">
-        <f>G5*(H$3/$G$3)^2</f>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
+        <f>H5*(J$3/$H$3)^2</f>
         <v>76.5625</v>
       </c>
-      <c r="I5" s="6">
-        <f>G5*(I$3/$G$3)^2</f>
+      <c r="K5" s="6">
+        <f>H5*(K$3/$H$3)^2</f>
         <v>9.765625</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5">
-        <f>D6*(E$3/$D$3)^2</f>
-        <v>0</v>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1000000</v>
       </c>
       <c r="F6" s="5">
-        <f>$D6*(F$3/$D$3)^2</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5">
-        <f>G6*(H$3/$G$3)^2</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <f>G6*(I$3/$G$3)^2</f>
-        <v>0</v>
+        <f>E6*(F$3/$E$3)^2</f>
+        <v>765625</v>
+      </c>
+      <c r="G6" s="5">
+        <f>$E6*(G$3/$E$3)^2</f>
+        <v>97656.25</v>
+      </c>
+      <c r="I6" s="5">
+        <v>48</v>
+      </c>
+      <c r="J6" s="5">
+        <f>I6*(J$3/$I$3)^2</f>
+        <v>36.75</v>
+      </c>
+      <c r="K6" s="6">
+        <f>I6*(K$3/$I$3)^2</f>
+        <v>4.6875</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8">
-        <f>D7*(E$3/$D$3)^2</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <f>$D7*(F$3/$D$3)^2</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8">
-        <f>G7*(H$3/$G$3)^2</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <f>G7*(I$3/$G$3)^2</f>
-        <v>0</v>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
+      <c r="C7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>54288</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7">
+        <f>D7*(F$3/$D$3)^2</f>
+        <v>10391.0625</v>
+      </c>
+      <c r="G7" s="7">
+        <f>$D7*(G$3/$D$3)^2</f>
+        <v>1325.390625</v>
+      </c>
+      <c r="H7" s="7">
+        <v>34</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7">
+        <f>H7*(J$3/$H$3)^2</f>
+        <v>6.5078125</v>
+      </c>
+      <c r="K7" s="8">
+        <f>H7*(K$3/$H$3)^2</f>
+        <v>0.830078125</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="D2:G2"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>